<commit_message>
worked for a sample...
</commit_message>
<xml_diff>
--- a/src/lithium/data/La Compil des data isotopes pour Yann 12-11-2018.xlsx
+++ b/src/lithium/data/La Compil des data isotopes pour Yann 12-11-2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="35200" windowHeight="20380" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="35260" windowHeight="20380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -488,8 +488,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="235">
+  <cellStyleXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -903,7 +905,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="235">
+  <cellStyles count="237">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1021,6 +1023,7 @@
     <cellStyle name="Lien hypertexte" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1138,6 +1141,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3949,7 +3953,7 @@
   <dimension ref="A1:AC159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="H14" sqref="H14:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>